<commit_message>
feat : Cleaned dataset.
Removed unwanted columns for the analysis.
Fill null in records which where to be zero
</commit_message>
<xml_diff>
--- a/datatype.xlsx
+++ b/datatype.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Documents\Data Science Tranings\Udacity Nanodegree\Prosper Loan Data Exploratory analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB837D1C-3030-45A5-B4FE-5C2B92CC5BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0017D86D-20AC-475C-B607-F29522DE59FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1E5D1BE2-8246-4985-B245-A58A5B942A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$81</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="96">
   <si>
     <t>non-null</t>
   </si>
@@ -314,6 +317,15 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -665,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAEB30E-3743-4BC5-B27E-AC790968AD1A}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,15 +691,18 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -697,8 +712,11 @@
       <c r="D2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -708,8 +726,11 @@
       <c r="D3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -720,7 +741,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -728,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -739,7 +760,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -749,8 +770,11 @@
       <c r="D7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -758,7 +782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -766,7 +790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -774,7 +798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -782,7 +806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -790,7 +814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -798,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -811,8 +835,11 @@
       <c r="D14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -826,7 +853,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -834,7 +861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -848,7 +875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -856,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -864,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -875,15 +902,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -891,23 +921,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -917,24 +953,33 @@
       <c r="D25" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -944,8 +989,11 @@
       <c r="D28" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -955,8 +1003,11 @@
       <c r="D29" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -966,8 +1017,11 @@
       <c r="D30" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -977,16 +1031,22 @@
       <c r="D31" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -996,8 +1056,11 @@
       <c r="D33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1007,24 +1070,36 @@
       <c r="D34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1032,47 +1107,68 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1080,15 +1176,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1098,16 +1200,28 @@
       <c r="C45" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -1115,7 +1229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -1123,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1131,7 +1245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1139,55 +1253,73 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>53</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>55</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>57</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1195,7 +1327,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -1203,7 +1335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -1211,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -1219,63 +1351,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>63</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>92</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>66</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>69</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -1283,71 +1445,95 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>71</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>72</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -1355,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -1363,7 +1549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -1371,7 +1557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -1388,6 +1574,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E81" xr:uid="{3DAEB30E-3743-4BC5-B27E-AC790968AD1A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>